<commit_message>
fix household model excel template
</commit_message>
<xml_diff>
--- a/input_data/excel_templates/household_template.xlsx
+++ b/input_data/excel_templates/household_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects_c\population_projections_c\input_data\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEB1817-FD4D-4B6F-9669-C063E453A982}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8646E917-6B2F-4104-847C-A00C2CAFCD20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12450" yWindow="-345" windowWidth="15390" windowHeight="9533" xr2:uid="{8ADEF3A0-FDEC-49D7-A33D-597C5EA6E207}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{8ADEF3A0-FDEC-49D7-A33D-597C5EA6E207}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>sex</t>
   </si>
@@ -92,15 +92,6 @@
     <t>demography@london.gov.uk</t>
   </si>
   <si>
-    <t>London Borough household projections DCLG Model</t>
-  </si>
-  <si>
-    <t>to households using the 2014 DCLG Household Model</t>
-  </si>
-  <si>
-    <t>2. Communal establishment populations are taken from the 2014 DCLG household model</t>
-  </si>
-  <si>
     <t>gss code</t>
   </si>
   <si>
@@ -120,6 +111,15 @@
   </si>
   <si>
     <t>average household size</t>
+  </si>
+  <si>
+    <t>London Borough household projections ONS Model</t>
+  </si>
+  <si>
+    <t>to households using the 2016 ONS Household Model</t>
+  </si>
+  <si>
+    <t>2. Communal establishment populations are taken from the 2016 ONS household model</t>
   </si>
 </sst>
 </file>
@@ -510,9 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375C0576-7F7E-4343-A918-FF609D82B2DD}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -526,7 +524,7 @@
     </row>
     <row r="2" spans="1:1" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5"/>
@@ -547,7 +545,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
@@ -567,7 +565,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
@@ -617,7 +615,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030A77D6-E931-4866-8F0C-C50F520B68E6}">
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -625,143 +623,139 @@
   <cols>
     <col min="1" max="1" width="11.06640625" customWidth="1"/>
     <col min="2" max="2" width="21.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="E1" s="4">
+        <v>2011</v>
       </c>
       <c r="F1" s="4">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="G1" s="4">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="H1" s="4">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="I1" s="4">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="J1" s="4">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="K1" s="4">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="L1" s="4">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="M1" s="4">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="N1" s="4">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="O1" s="4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P1" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="Q1" s="4">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="R1" s="4">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="S1" s="4">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="T1" s="4">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="U1" s="4">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="V1" s="4">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="W1" s="4">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="X1" s="4">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="Y1" s="4">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="Z1" s="4">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="AA1" s="4">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="AB1" s="4">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="AC1" s="4">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="AD1" s="4">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="AE1" s="4">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="AF1" s="4">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="AG1" s="4">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="AH1" s="4">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="AI1" s="4">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="AJ1" s="4">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="AK1" s="4">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="AL1" s="4">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="AM1" s="4">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="AN1" s="4">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AO1" s="4">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AP1" s="4">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AQ1" s="4">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AR1" s="4">
-        <v>2049</v>
-      </c>
-      <c r="AS1" s="4">
         <v>2050</v>
       </c>
     </row>
@@ -785,16 +779,16 @@
   <sheetData>
     <row r="1" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E1" s="4">
         <v>2011</v>
@@ -936,16 +930,16 @@
   <sheetData>
     <row r="1" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="4">
         <v>2011</v>
@@ -1087,16 +1081,16 @@
   <sheetData>
     <row r="1" spans="1:44" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="4">
         <v>2011</v>
@@ -1240,10 +1234,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -1252,13 +1246,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>